<commit_message>
Added contiguous mosaics. Added Don't Panic test page for contiguous mosaics.
</commit_message>
<xml_diff>
--- a/docs/control codes.xlsx
+++ b/docs/control codes.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robin\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robin\Documents\Visual Studio 2015\Projects\NexTel\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D89BF285-65F3-4EE9-BD26-98824874A261}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FF67584-EC3F-4EB9-82CA-D93A813EFA5A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16695" windowHeight="5955" activeTab="1" xr2:uid="{1D35677F-1048-41AB-9A0D-5C34EC10B2B0}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16695" windowHeight="5955" xr2:uid="{1D35677F-1048-41AB-9A0D-5C34EC10B2B0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -139,8 +139,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -455,18 +458,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B0846F3-C267-499B-9941-B9FBFB633FBE}">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>129</v>
       </c>
@@ -477,8 +481,12 @@
         <f>DEC2BIN(A1, 8)</f>
         <v>10000001</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="1" t="str">
+        <f>DEC2HEX(A1)</f>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>130</v>
       </c>
@@ -489,8 +497,12 @@
         <f t="shared" ref="C2:C25" si="0">DEC2BIN(A2, 8)</f>
         <v>10000010</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" s="1" t="str">
+        <f t="shared" ref="D2:D25" si="1">DEC2HEX(A2)</f>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>131</v>
       </c>
@@ -501,8 +513,12 @@
         <f t="shared" si="0"/>
         <v>10000011</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>132</v>
       </c>
@@ -513,8 +529,12 @@
         <f t="shared" si="0"/>
         <v>10000100</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>133</v>
       </c>
@@ -525,8 +545,12 @@
         <f t="shared" si="0"/>
         <v>10000101</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>134</v>
       </c>
@@ -537,8 +561,12 @@
         <f t="shared" si="0"/>
         <v>10000110</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>135</v>
       </c>
@@ -549,8 +577,12 @@
         <f t="shared" si="0"/>
         <v>10000111</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>87</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>136</v>
       </c>
@@ -561,8 +593,12 @@
         <f t="shared" si="0"/>
         <v>10001000</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>137</v>
       </c>
@@ -573,8 +609,12 @@
         <f t="shared" si="0"/>
         <v>10001001</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>140</v>
       </c>
@@ -585,8 +625,12 @@
         <f t="shared" si="0"/>
         <v>10001100</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>8C</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>141</v>
       </c>
@@ -597,8 +641,12 @@
         <f t="shared" si="0"/>
         <v>10001101</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>8D</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>145</v>
       </c>
@@ -609,8 +657,12 @@
         <f t="shared" si="0"/>
         <v>10010001</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>91</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>146</v>
       </c>
@@ -621,8 +673,12 @@
         <f t="shared" si="0"/>
         <v>10010010</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>92</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>147</v>
       </c>
@@ -633,8 +689,12 @@
         <f t="shared" si="0"/>
         <v>10010011</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>148</v>
       </c>
@@ -645,8 +705,12 @@
         <f t="shared" si="0"/>
         <v>10010100</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D15" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>94</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>149</v>
       </c>
@@ -657,8 +721,12 @@
         <f t="shared" si="0"/>
         <v>10010101</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>150</v>
       </c>
@@ -669,8 +737,12 @@
         <f t="shared" si="0"/>
         <v>10010110</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>151</v>
       </c>
@@ -681,8 +753,12 @@
         <f t="shared" si="0"/>
         <v>10010111</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>97</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>152</v>
       </c>
@@ -693,8 +769,12 @@
         <f t="shared" si="0"/>
         <v>10011000</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>98</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>153</v>
       </c>
@@ -705,8 +785,12 @@
         <f t="shared" si="0"/>
         <v>10011001</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>154</v>
       </c>
@@ -717,8 +801,12 @@
         <f t="shared" si="0"/>
         <v>10011010</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D21" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>9A</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>156</v>
       </c>
@@ -729,8 +817,12 @@
         <f t="shared" si="0"/>
         <v>10011100</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D22" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>9C</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>157</v>
       </c>
@@ -741,8 +833,12 @@
         <f t="shared" si="0"/>
         <v>10011101</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D23" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>9D</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>158</v>
       </c>
@@ -753,8 +849,12 @@
         <f t="shared" si="0"/>
         <v>10011110</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D24" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>9E</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>159</v>
       </c>
@@ -764,6 +864,10 @@
       <c r="C25" t="str">
         <f t="shared" si="0"/>
         <v>10011111</v>
+      </c>
+      <c r="D25" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>9F</v>
       </c>
     </row>
   </sheetData>
@@ -775,8 +879,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{804CB660-8CFB-4F70-B751-D2BBCE3FAF4B}">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added coloured backgrounds. Completed double height font.
</commit_message>
<xml_diff>
--- a/docs/control codes.xlsx
+++ b/docs/control codes.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robin\Documents\Visual Studio 2015\Projects\NexTel\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E53032A-81B2-408C-A717-A684E28A2B26}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C888221-73A8-423D-8251-4913A6BE69BB}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16695" windowHeight="5955" activeTab="1" xr2:uid="{1D35677F-1048-41AB-9A0D-5C34EC10B2B0}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16695" windowHeight="5955" xr2:uid="{1D35677F-1048-41AB-9A0D-5C34EC10B2B0}"/>
   </bookViews>
   <sheets>
-    <sheet name="CtrlCodes" sheetId="1" r:id="rId1"/>
-    <sheet name="Graphics" sheetId="3" r:id="rId2"/>
-    <sheet name="Test" sheetId="2" r:id="rId3"/>
+    <sheet name="Colours" sheetId="4" r:id="rId1"/>
+    <sheet name="CtrlCodes" sheetId="1" r:id="rId2"/>
+    <sheet name="Graphics" sheetId="3" r:id="rId3"/>
+    <sheet name="Test" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="101">
   <si>
     <t>alphanumeric red</t>
   </si>
@@ -207,13 +208,136 @@
   </si>
   <si>
     <t>DF</t>
+  </si>
+  <si>
+    <t>White</t>
+  </si>
+  <si>
+    <t>Cyan</t>
+  </si>
+  <si>
+    <t>Magenta</t>
+  </si>
+  <si>
+    <t>Blue</t>
+  </si>
+  <si>
+    <t>Yellow</t>
+  </si>
+  <si>
+    <t>Green</t>
+  </si>
+  <si>
+    <t>Red</t>
+  </si>
+  <si>
+    <t>Black</t>
+  </si>
+  <si>
+    <t>STEADY foreground when background is BLACK</t>
+  </si>
+  <si>
+    <t>STEADY foreground when background is RED</t>
+  </si>
+  <si>
+    <t>STEADY foreground when background is GREEN</t>
+  </si>
+  <si>
+    <t>STEADY foreground when background is YELLOW</t>
+  </si>
+  <si>
+    <t>STEADY foreground when background is BLUE</t>
+  </si>
+  <si>
+    <t>STEADY foreground when background is MAGENTA</t>
+  </si>
+  <si>
+    <t>STEADY foreground when background is CYAN</t>
+  </si>
+  <si>
+    <t>STEADY foreground when background is WHITE</t>
+  </si>
+  <si>
+    <t>FLASHING foreground when background is BLACK</t>
+  </si>
+  <si>
+    <t>FLASHING foreground when background is RED</t>
+  </si>
+  <si>
+    <t>FLASHING foreground when background is GREEN</t>
+  </si>
+  <si>
+    <t>FLASHING foreground when background is YELLOW</t>
+  </si>
+  <si>
+    <t>FLASHING foreground when background is BLUE</t>
+  </si>
+  <si>
+    <t>FLASHING foreground when background is MAGENTA</t>
+  </si>
+  <si>
+    <t>FLASHING foreground when background is CYAN</t>
+  </si>
+  <si>
+    <t>FLASHING foreground when background is WHITE</t>
+  </si>
+  <si>
+    <t>To</t>
+  </si>
+  <si>
+    <t>From</t>
+  </si>
+  <si>
+    <t>Bit 7</t>
+  </si>
+  <si>
+    <t>Bits 0..2</t>
+  </si>
+  <si>
+    <t>Bits 3..5</t>
+  </si>
+  <si>
+    <t>Bit 6</t>
+  </si>
+  <si>
+    <t>BG of FG</t>
+  </si>
+  <si>
+    <t>Is Flash?</t>
+  </si>
+  <si>
+    <t>Is BG?</t>
+  </si>
+  <si>
+    <t>Colour</t>
+  </si>
+  <si>
+    <t>Foreground:</t>
+  </si>
+  <si>
+    <t>Background:</t>
+  </si>
+  <si>
+    <t>(FG Colour) OR (BG Colour &lt;&lt; 3) OR (Flashing &lt;&lt; 6)</t>
+  </si>
+  <si>
+    <t>(BG Colour) OR (128)</t>
+  </si>
+  <si>
+    <t>Palette indices 136..255 are not used, except $E3 which is transparent (for box mode support)</t>
+  </si>
+  <si>
+    <t>Conceal/Reveal is implemented by substituting Conceal $98 for Escape $9B (or vice-versa) in the buffer, then re-rendering</t>
+  </si>
+  <si>
+    <t>Box mode is implemented by rendering with a branch to draw transparent FG and BG when outside box</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -266,13 +390,144 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0" tint="-0.34998626667073579"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF00CCFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF00FF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF9933"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF008000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF008000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0000FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF00FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00CCFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -287,7 +542,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -328,12 +583,101 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF008000"/>
+      <color rgb="FFFFCC00"/>
+      <color rgb="FFFF9933"/>
+      <color rgb="FF0000FF"/>
+      <color rgb="FFFF00FF"/>
+      <color rgb="FF00CCFF"/>
+      <color rgb="FF339933"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -641,6 +985,1697 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E06C7C1-2502-41BC-8AA4-E8D6C1F363EE}">
+  <dimension ref="A1:W33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="9" width="4" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="17" width="11.85546875" style="1" customWidth="1"/>
+    <col min="18" max="19" width="9" style="39" bestFit="1" customWidth="1"/>
+    <col min="20" max="23" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3"/>
+      <c r="B1" s="3">
+        <v>7</v>
+      </c>
+      <c r="C1" s="3">
+        <f>B1-1</f>
+        <v>6</v>
+      </c>
+      <c r="D1" s="3">
+        <f t="shared" ref="D1:I1" si="0">C1-1</f>
+        <v>5</v>
+      </c>
+      <c r="E1" s="3">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="F1" s="3">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="G1" s="3">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="H1" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I1" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J1" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="K1" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="L1" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="M1" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="N1" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="O1" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="P1" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="R1" s="30" t="s">
+        <v>84</v>
+      </c>
+      <c r="S1" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="T1" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="U1" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="V1" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="W1" s="10" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
+        <v>0</v>
+      </c>
+      <c r="B2" s="11">
+        <f>($A2 * 8) + B$1</f>
+        <v>7</v>
+      </c>
+      <c r="C2" s="11">
+        <f t="shared" ref="C2:I17" si="1">($A2 * 8) + C$1</f>
+        <v>6</v>
+      </c>
+      <c r="D2" s="11">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="E2" s="11">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="F2" s="11">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="G2" s="11">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="H2" s="11">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I2" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J2" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="K2" s="22"/>
+      <c r="L2" s="22"/>
+      <c r="M2" s="22"/>
+      <c r="N2" s="22"/>
+      <c r="O2" s="22"/>
+      <c r="P2" s="22"/>
+      <c r="Q2" s="22"/>
+      <c r="R2" s="39" t="str">
+        <f>DEC2BIN(B2, 8)</f>
+        <v>00000111</v>
+      </c>
+      <c r="S2" s="39" t="str">
+        <f>DEC2BIN(I2, 8)</f>
+        <v>00000000</v>
+      </c>
+      <c r="T2" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="U2" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="V2" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="W2" s="11" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <f>A2+1</f>
+        <v>1</v>
+      </c>
+      <c r="B3" s="11">
+        <f t="shared" ref="B3:I18" si="2">($A3 * 8) + B$1</f>
+        <v>15</v>
+      </c>
+      <c r="C3" s="11">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="D3" s="11">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="E3" s="11">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="F3" s="11">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="G3" s="11">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="H3" s="11">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="I3" s="11">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="J3" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="K3" s="23"/>
+      <c r="L3" s="23"/>
+      <c r="M3" s="23"/>
+      <c r="N3" s="23"/>
+      <c r="O3" s="23"/>
+      <c r="P3" s="23"/>
+      <c r="Q3" s="23"/>
+      <c r="R3" s="39" t="str">
+        <f t="shared" ref="R3:R18" si="3">DEC2BIN(B3, 8)</f>
+        <v>00001111</v>
+      </c>
+      <c r="S3" s="39" t="str">
+        <f t="shared" ref="S3:S18" si="4">DEC2BIN(I3, 8)</f>
+        <v>00001000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <f t="shared" ref="A4:A33" si="5">A3+1</f>
+        <v>2</v>
+      </c>
+      <c r="B4" s="11">
+        <f t="shared" si="2"/>
+        <v>23</v>
+      </c>
+      <c r="C4" s="11">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="D4" s="11">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+      <c r="E4" s="11">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="F4" s="11">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="G4" s="11">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="H4" s="11">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="I4" s="11">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="J4" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="K4" s="24"/>
+      <c r="L4" s="24"/>
+      <c r="M4" s="24"/>
+      <c r="N4" s="24"/>
+      <c r="O4" s="24"/>
+      <c r="P4" s="24"/>
+      <c r="Q4" s="24"/>
+      <c r="R4" s="39" t="str">
+        <f t="shared" si="3"/>
+        <v>00010111</v>
+      </c>
+      <c r="S4" s="39" t="str">
+        <f t="shared" si="4"/>
+        <v>00010000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="B5" s="11">
+        <f t="shared" si="2"/>
+        <v>31</v>
+      </c>
+      <c r="C5" s="11">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="D5" s="11">
+        <f t="shared" si="1"/>
+        <v>29</v>
+      </c>
+      <c r="E5" s="11">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+      <c r="F5" s="11">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
+      <c r="G5" s="11">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+      <c r="H5" s="11">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="I5" s="11">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="J5" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="K5" s="25"/>
+      <c r="L5" s="25"/>
+      <c r="M5" s="25"/>
+      <c r="N5" s="25"/>
+      <c r="O5" s="25"/>
+      <c r="P5" s="25"/>
+      <c r="Q5" s="25"/>
+      <c r="R5" s="39" t="str">
+        <f t="shared" si="3"/>
+        <v>00011111</v>
+      </c>
+      <c r="S5" s="39" t="str">
+        <f t="shared" si="4"/>
+        <v>00011000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="B6" s="11">
+        <f t="shared" si="2"/>
+        <v>39</v>
+      </c>
+      <c r="C6" s="11">
+        <f t="shared" si="1"/>
+        <v>38</v>
+      </c>
+      <c r="D6" s="11">
+        <f t="shared" si="1"/>
+        <v>37</v>
+      </c>
+      <c r="E6" s="11">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+      <c r="F6" s="11">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+      <c r="G6" s="11">
+        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
+      <c r="H6" s="11">
+        <f t="shared" si="1"/>
+        <v>33</v>
+      </c>
+      <c r="I6" s="11">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+      <c r="J6" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="K6" s="26"/>
+      <c r="L6" s="26"/>
+      <c r="M6" s="26"/>
+      <c r="N6" s="26"/>
+      <c r="O6" s="26"/>
+      <c r="P6" s="26"/>
+      <c r="Q6" s="26"/>
+      <c r="R6" s="39" t="str">
+        <f t="shared" si="3"/>
+        <v>00100111</v>
+      </c>
+      <c r="S6" s="39" t="str">
+        <f t="shared" si="4"/>
+        <v>00100000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="B7" s="11">
+        <f t="shared" si="2"/>
+        <v>47</v>
+      </c>
+      <c r="C7" s="11">
+        <f t="shared" si="1"/>
+        <v>46</v>
+      </c>
+      <c r="D7" s="11">
+        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
+      <c r="E7" s="11">
+        <f t="shared" si="1"/>
+        <v>44</v>
+      </c>
+      <c r="F7" s="11">
+        <f t="shared" si="1"/>
+        <v>43</v>
+      </c>
+      <c r="G7" s="11">
+        <f t="shared" si="1"/>
+        <v>42</v>
+      </c>
+      <c r="H7" s="11">
+        <f t="shared" si="1"/>
+        <v>41</v>
+      </c>
+      <c r="I7" s="11">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="J7" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="K7" s="27"/>
+      <c r="L7" s="27"/>
+      <c r="M7" s="27"/>
+      <c r="N7" s="27"/>
+      <c r="O7" s="27"/>
+      <c r="P7" s="27"/>
+      <c r="Q7" s="27"/>
+      <c r="R7" s="39" t="str">
+        <f t="shared" si="3"/>
+        <v>00101111</v>
+      </c>
+      <c r="S7" s="39" t="str">
+        <f t="shared" si="4"/>
+        <v>00101000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="B8" s="11">
+        <f t="shared" si="2"/>
+        <v>55</v>
+      </c>
+      <c r="C8" s="11">
+        <f t="shared" si="1"/>
+        <v>54</v>
+      </c>
+      <c r="D8" s="11">
+        <f t="shared" si="1"/>
+        <v>53</v>
+      </c>
+      <c r="E8" s="11">
+        <f t="shared" si="1"/>
+        <v>52</v>
+      </c>
+      <c r="F8" s="11">
+        <f t="shared" si="1"/>
+        <v>51</v>
+      </c>
+      <c r="G8" s="11">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="H8" s="11">
+        <f t="shared" si="1"/>
+        <v>49</v>
+      </c>
+      <c r="I8" s="11">
+        <f t="shared" si="1"/>
+        <v>48</v>
+      </c>
+      <c r="J8" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="K8" s="28"/>
+      <c r="L8" s="28"/>
+      <c r="M8" s="28"/>
+      <c r="N8" s="28"/>
+      <c r="O8" s="28"/>
+      <c r="P8" s="28"/>
+      <c r="Q8" s="28"/>
+      <c r="R8" s="39" t="str">
+        <f t="shared" si="3"/>
+        <v>00110111</v>
+      </c>
+      <c r="S8" s="39" t="str">
+        <f t="shared" si="4"/>
+        <v>00110000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <f t="shared" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="B9" s="11">
+        <f t="shared" si="2"/>
+        <v>63</v>
+      </c>
+      <c r="C9" s="11">
+        <f t="shared" si="1"/>
+        <v>62</v>
+      </c>
+      <c r="D9" s="11">
+        <f t="shared" si="1"/>
+        <v>61</v>
+      </c>
+      <c r="E9" s="11">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+      <c r="F9" s="11">
+        <f t="shared" si="1"/>
+        <v>59</v>
+      </c>
+      <c r="G9" s="11">
+        <f t="shared" si="1"/>
+        <v>58</v>
+      </c>
+      <c r="H9" s="11">
+        <f t="shared" si="1"/>
+        <v>57</v>
+      </c>
+      <c r="I9" s="11">
+        <f t="shared" si="1"/>
+        <v>56</v>
+      </c>
+      <c r="J9" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="K9" s="29"/>
+      <c r="L9" s="29"/>
+      <c r="M9" s="29"/>
+      <c r="N9" s="29"/>
+      <c r="O9" s="29"/>
+      <c r="P9" s="29"/>
+      <c r="Q9" s="29"/>
+      <c r="R9" s="39" t="str">
+        <f t="shared" si="3"/>
+        <v>00111111</v>
+      </c>
+      <c r="S9" s="39" t="str">
+        <f t="shared" si="4"/>
+        <v>00111000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="B10" s="11">
+        <f t="shared" si="2"/>
+        <v>71</v>
+      </c>
+      <c r="C10" s="11">
+        <f t="shared" si="1"/>
+        <v>70</v>
+      </c>
+      <c r="D10" s="11">
+        <f t="shared" si="1"/>
+        <v>69</v>
+      </c>
+      <c r="E10" s="11">
+        <f t="shared" si="1"/>
+        <v>68</v>
+      </c>
+      <c r="F10" s="11">
+        <f t="shared" si="1"/>
+        <v>67</v>
+      </c>
+      <c r="G10" s="11">
+        <f t="shared" si="1"/>
+        <v>66</v>
+      </c>
+      <c r="H10" s="11">
+        <f t="shared" si="1"/>
+        <v>65</v>
+      </c>
+      <c r="I10" s="11">
+        <f t="shared" si="1"/>
+        <v>64</v>
+      </c>
+      <c r="J10" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="K10" s="22"/>
+      <c r="L10" s="22"/>
+      <c r="M10" s="22"/>
+      <c r="N10" s="22"/>
+      <c r="O10" s="22"/>
+      <c r="P10" s="22"/>
+      <c r="Q10" s="22"/>
+      <c r="R10" s="39" t="str">
+        <f t="shared" si="3"/>
+        <v>01000111</v>
+      </c>
+      <c r="S10" s="39" t="str">
+        <f t="shared" si="4"/>
+        <v>01000000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
+      <c r="B11" s="11">
+        <f t="shared" si="2"/>
+        <v>79</v>
+      </c>
+      <c r="C11" s="11">
+        <f t="shared" si="1"/>
+        <v>78</v>
+      </c>
+      <c r="D11" s="11">
+        <f t="shared" si="1"/>
+        <v>77</v>
+      </c>
+      <c r="E11" s="11">
+        <f t="shared" si="1"/>
+        <v>76</v>
+      </c>
+      <c r="F11" s="11">
+        <f t="shared" si="1"/>
+        <v>75</v>
+      </c>
+      <c r="G11" s="11">
+        <f t="shared" si="1"/>
+        <v>74</v>
+      </c>
+      <c r="H11" s="11">
+        <f t="shared" si="1"/>
+        <v>73</v>
+      </c>
+      <c r="I11" s="11">
+        <f t="shared" si="1"/>
+        <v>72</v>
+      </c>
+      <c r="J11" s="23" t="s">
+        <v>77</v>
+      </c>
+      <c r="K11" s="23"/>
+      <c r="L11" s="23"/>
+      <c r="M11" s="23"/>
+      <c r="N11" s="23"/>
+      <c r="O11" s="23"/>
+      <c r="P11" s="23"/>
+      <c r="Q11" s="23"/>
+      <c r="R11" s="39" t="str">
+        <f t="shared" si="3"/>
+        <v>01001111</v>
+      </c>
+      <c r="S11" s="39" t="str">
+        <f t="shared" si="4"/>
+        <v>01001000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="B12" s="11">
+        <f t="shared" si="2"/>
+        <v>87</v>
+      </c>
+      <c r="C12" s="11">
+        <f t="shared" si="1"/>
+        <v>86</v>
+      </c>
+      <c r="D12" s="11">
+        <f t="shared" si="1"/>
+        <v>85</v>
+      </c>
+      <c r="E12" s="11">
+        <f t="shared" si="1"/>
+        <v>84</v>
+      </c>
+      <c r="F12" s="11">
+        <f t="shared" si="1"/>
+        <v>83</v>
+      </c>
+      <c r="G12" s="11">
+        <f t="shared" si="1"/>
+        <v>82</v>
+      </c>
+      <c r="H12" s="11">
+        <f t="shared" si="1"/>
+        <v>81</v>
+      </c>
+      <c r="I12" s="11">
+        <f t="shared" si="1"/>
+        <v>80</v>
+      </c>
+      <c r="J12" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="K12" s="24"/>
+      <c r="L12" s="24"/>
+      <c r="M12" s="24"/>
+      <c r="N12" s="24"/>
+      <c r="O12" s="24"/>
+      <c r="P12" s="24"/>
+      <c r="Q12" s="24"/>
+      <c r="R12" s="39" t="str">
+        <f t="shared" si="3"/>
+        <v>01010111</v>
+      </c>
+      <c r="S12" s="39" t="str">
+        <f t="shared" si="4"/>
+        <v>01010000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
+        <f t="shared" si="5"/>
+        <v>11</v>
+      </c>
+      <c r="B13" s="11">
+        <f t="shared" si="2"/>
+        <v>95</v>
+      </c>
+      <c r="C13" s="11">
+        <f t="shared" si="1"/>
+        <v>94</v>
+      </c>
+      <c r="D13" s="11">
+        <f t="shared" si="1"/>
+        <v>93</v>
+      </c>
+      <c r="E13" s="11">
+        <f t="shared" si="1"/>
+        <v>92</v>
+      </c>
+      <c r="F13" s="11">
+        <f t="shared" si="1"/>
+        <v>91</v>
+      </c>
+      <c r="G13" s="11">
+        <f t="shared" si="1"/>
+        <v>90</v>
+      </c>
+      <c r="H13" s="11">
+        <f t="shared" si="1"/>
+        <v>89</v>
+      </c>
+      <c r="I13" s="11">
+        <f t="shared" si="1"/>
+        <v>88</v>
+      </c>
+      <c r="J13" s="25" t="s">
+        <v>79</v>
+      </c>
+      <c r="K13" s="25"/>
+      <c r="L13" s="25"/>
+      <c r="M13" s="25"/>
+      <c r="N13" s="25"/>
+      <c r="O13" s="25"/>
+      <c r="P13" s="25"/>
+      <c r="Q13" s="25"/>
+      <c r="R13" s="39" t="str">
+        <f t="shared" si="3"/>
+        <v>01011111</v>
+      </c>
+      <c r="S13" s="39" t="str">
+        <f t="shared" si="4"/>
+        <v>01011000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
+        <f t="shared" si="5"/>
+        <v>12</v>
+      </c>
+      <c r="B14" s="11">
+        <f t="shared" si="2"/>
+        <v>103</v>
+      </c>
+      <c r="C14" s="11">
+        <f t="shared" si="1"/>
+        <v>102</v>
+      </c>
+      <c r="D14" s="11">
+        <f t="shared" si="1"/>
+        <v>101</v>
+      </c>
+      <c r="E14" s="11">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="F14" s="11">
+        <f t="shared" si="1"/>
+        <v>99</v>
+      </c>
+      <c r="G14" s="11">
+        <f t="shared" si="1"/>
+        <v>98</v>
+      </c>
+      <c r="H14" s="11">
+        <f t="shared" si="1"/>
+        <v>97</v>
+      </c>
+      <c r="I14" s="11">
+        <f t="shared" si="1"/>
+        <v>96</v>
+      </c>
+      <c r="J14" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="K14" s="26"/>
+      <c r="L14" s="26"/>
+      <c r="M14" s="26"/>
+      <c r="N14" s="26"/>
+      <c r="O14" s="26"/>
+      <c r="P14" s="26"/>
+      <c r="Q14" s="26"/>
+      <c r="R14" s="39" t="str">
+        <f t="shared" si="3"/>
+        <v>01100111</v>
+      </c>
+      <c r="S14" s="39" t="str">
+        <f t="shared" si="4"/>
+        <v>01100000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A15" s="3">
+        <f t="shared" si="5"/>
+        <v>13</v>
+      </c>
+      <c r="B15" s="11">
+        <f t="shared" si="2"/>
+        <v>111</v>
+      </c>
+      <c r="C15" s="11">
+        <f t="shared" si="1"/>
+        <v>110</v>
+      </c>
+      <c r="D15" s="11">
+        <f t="shared" si="1"/>
+        <v>109</v>
+      </c>
+      <c r="E15" s="11">
+        <f t="shared" si="1"/>
+        <v>108</v>
+      </c>
+      <c r="F15" s="11">
+        <f t="shared" si="1"/>
+        <v>107</v>
+      </c>
+      <c r="G15" s="11">
+        <f t="shared" si="1"/>
+        <v>106</v>
+      </c>
+      <c r="H15" s="11">
+        <f t="shared" si="1"/>
+        <v>105</v>
+      </c>
+      <c r="I15" s="11">
+        <f t="shared" si="1"/>
+        <v>104</v>
+      </c>
+      <c r="J15" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="K15" s="27"/>
+      <c r="L15" s="27"/>
+      <c r="M15" s="27"/>
+      <c r="N15" s="27"/>
+      <c r="O15" s="27"/>
+      <c r="P15" s="27"/>
+      <c r="Q15" s="27"/>
+      <c r="R15" s="39" t="str">
+        <f t="shared" si="3"/>
+        <v>01101111</v>
+      </c>
+      <c r="S15" s="39" t="str">
+        <f t="shared" si="4"/>
+        <v>01101000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A16" s="3">
+        <f t="shared" si="5"/>
+        <v>14</v>
+      </c>
+      <c r="B16" s="11">
+        <f t="shared" si="2"/>
+        <v>119</v>
+      </c>
+      <c r="C16" s="11">
+        <f t="shared" si="1"/>
+        <v>118</v>
+      </c>
+      <c r="D16" s="11">
+        <f t="shared" si="1"/>
+        <v>117</v>
+      </c>
+      <c r="E16" s="11">
+        <f t="shared" si="1"/>
+        <v>116</v>
+      </c>
+      <c r="F16" s="11">
+        <f t="shared" si="1"/>
+        <v>115</v>
+      </c>
+      <c r="G16" s="11">
+        <f t="shared" si="1"/>
+        <v>114</v>
+      </c>
+      <c r="H16" s="11">
+        <f t="shared" si="1"/>
+        <v>113</v>
+      </c>
+      <c r="I16" s="11">
+        <f t="shared" si="1"/>
+        <v>112</v>
+      </c>
+      <c r="J16" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="K16" s="28"/>
+      <c r="L16" s="28"/>
+      <c r="M16" s="28"/>
+      <c r="N16" s="28"/>
+      <c r="O16" s="28"/>
+      <c r="P16" s="28"/>
+      <c r="Q16" s="28"/>
+      <c r="R16" s="39" t="str">
+        <f t="shared" si="3"/>
+        <v>01110111</v>
+      </c>
+      <c r="S16" s="39" t="str">
+        <f t="shared" si="4"/>
+        <v>01110000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A17" s="3">
+        <f t="shared" si="5"/>
+        <v>15</v>
+      </c>
+      <c r="B17" s="11">
+        <f t="shared" si="2"/>
+        <v>127</v>
+      </c>
+      <c r="C17" s="11">
+        <f t="shared" si="1"/>
+        <v>126</v>
+      </c>
+      <c r="D17" s="11">
+        <f t="shared" si="1"/>
+        <v>125</v>
+      </c>
+      <c r="E17" s="11">
+        <f t="shared" si="1"/>
+        <v>124</v>
+      </c>
+      <c r="F17" s="11">
+        <f t="shared" si="1"/>
+        <v>123</v>
+      </c>
+      <c r="G17" s="11">
+        <f t="shared" si="1"/>
+        <v>122</v>
+      </c>
+      <c r="H17" s="11">
+        <f t="shared" si="1"/>
+        <v>121</v>
+      </c>
+      <c r="I17" s="11">
+        <f t="shared" si="1"/>
+        <v>120</v>
+      </c>
+      <c r="J17" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="K17" s="29"/>
+      <c r="L17" s="29"/>
+      <c r="M17" s="29"/>
+      <c r="N17" s="29"/>
+      <c r="O17" s="29"/>
+      <c r="P17" s="29"/>
+      <c r="Q17" s="29"/>
+      <c r="R17" s="39" t="str">
+        <f t="shared" si="3"/>
+        <v>01111111</v>
+      </c>
+      <c r="S17" s="39" t="str">
+        <f t="shared" si="4"/>
+        <v>01111000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A18" s="3">
+        <f t="shared" si="5"/>
+        <v>16</v>
+      </c>
+      <c r="B18" s="11">
+        <f t="shared" si="2"/>
+        <v>135</v>
+      </c>
+      <c r="C18" s="11">
+        <f t="shared" si="2"/>
+        <v>134</v>
+      </c>
+      <c r="D18" s="11">
+        <f t="shared" si="2"/>
+        <v>133</v>
+      </c>
+      <c r="E18" s="11">
+        <f t="shared" si="2"/>
+        <v>132</v>
+      </c>
+      <c r="F18" s="11">
+        <f t="shared" si="2"/>
+        <v>131</v>
+      </c>
+      <c r="G18" s="11">
+        <f t="shared" si="2"/>
+        <v>130</v>
+      </c>
+      <c r="H18" s="11">
+        <f t="shared" si="2"/>
+        <v>129</v>
+      </c>
+      <c r="I18" s="11">
+        <f t="shared" si="2"/>
+        <v>128</v>
+      </c>
+      <c r="J18" s="31" t="str">
+        <f>J$1 &amp; " BG"</f>
+        <v>White BG</v>
+      </c>
+      <c r="K18" s="32" t="str">
+        <f t="shared" ref="K18:Q18" si="6">K$1 &amp; " BG"</f>
+        <v>Cyan BG</v>
+      </c>
+      <c r="L18" s="33" t="str">
+        <f t="shared" si="6"/>
+        <v>Magenta BG</v>
+      </c>
+      <c r="M18" s="34" t="str">
+        <f t="shared" si="6"/>
+        <v>Blue BG</v>
+      </c>
+      <c r="N18" s="35" t="str">
+        <f t="shared" si="6"/>
+        <v>Yellow BG</v>
+      </c>
+      <c r="O18" s="36" t="str">
+        <f t="shared" si="6"/>
+        <v>Green BG</v>
+      </c>
+      <c r="P18" s="37" t="str">
+        <f t="shared" si="6"/>
+        <v>Red BG</v>
+      </c>
+      <c r="Q18" s="38" t="str">
+        <f t="shared" si="6"/>
+        <v>Black BG</v>
+      </c>
+      <c r="R18" s="39" t="str">
+        <f t="shared" si="3"/>
+        <v>10000111</v>
+      </c>
+      <c r="S18" s="39" t="str">
+        <f t="shared" si="4"/>
+        <v>10000000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A19" s="3">
+        <f t="shared" si="5"/>
+        <v>17</v>
+      </c>
+      <c r="B19" s="11">
+        <f t="shared" ref="B19:I33" si="7">($A19 * 8) + B$1</f>
+        <v>143</v>
+      </c>
+      <c r="C19" s="11">
+        <f t="shared" si="7"/>
+        <v>142</v>
+      </c>
+      <c r="D19" s="11">
+        <f t="shared" si="7"/>
+        <v>141</v>
+      </c>
+      <c r="E19" s="11">
+        <f t="shared" si="7"/>
+        <v>140</v>
+      </c>
+      <c r="F19" s="11">
+        <f t="shared" si="7"/>
+        <v>139</v>
+      </c>
+      <c r="G19" s="11">
+        <f t="shared" si="7"/>
+        <v>138</v>
+      </c>
+      <c r="H19" s="11">
+        <f t="shared" si="7"/>
+        <v>137</v>
+      </c>
+      <c r="I19" s="11">
+        <f t="shared" si="7"/>
+        <v>136</v>
+      </c>
+      <c r="J19" s="40" t="s">
+        <v>94</v>
+      </c>
+      <c r="K19" s="41" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A20" s="3">
+        <f t="shared" si="5"/>
+        <v>18</v>
+      </c>
+      <c r="B20" s="11">
+        <f t="shared" si="7"/>
+        <v>151</v>
+      </c>
+      <c r="C20" s="11">
+        <f t="shared" si="7"/>
+        <v>150</v>
+      </c>
+      <c r="D20" s="11">
+        <f t="shared" si="7"/>
+        <v>149</v>
+      </c>
+      <c r="E20" s="11">
+        <f t="shared" si="7"/>
+        <v>148</v>
+      </c>
+      <c r="F20" s="11">
+        <f t="shared" si="7"/>
+        <v>147</v>
+      </c>
+      <c r="G20" s="11">
+        <f t="shared" si="7"/>
+        <v>146</v>
+      </c>
+      <c r="H20" s="11">
+        <f t="shared" si="7"/>
+        <v>145</v>
+      </c>
+      <c r="I20" s="11">
+        <f t="shared" si="7"/>
+        <v>144</v>
+      </c>
+      <c r="J20" s="40" t="s">
+        <v>95</v>
+      </c>
+      <c r="K20" s="41" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A21" s="3">
+        <f t="shared" si="5"/>
+        <v>19</v>
+      </c>
+      <c r="B21" s="11">
+        <f t="shared" si="7"/>
+        <v>159</v>
+      </c>
+      <c r="C21" s="11">
+        <f t="shared" si="7"/>
+        <v>158</v>
+      </c>
+      <c r="D21" s="11">
+        <f t="shared" si="7"/>
+        <v>157</v>
+      </c>
+      <c r="E21" s="11">
+        <f t="shared" si="7"/>
+        <v>156</v>
+      </c>
+      <c r="F21" s="11">
+        <f t="shared" si="7"/>
+        <v>155</v>
+      </c>
+      <c r="G21" s="11">
+        <f t="shared" si="7"/>
+        <v>154</v>
+      </c>
+      <c r="H21" s="11">
+        <f t="shared" si="7"/>
+        <v>153</v>
+      </c>
+      <c r="I21" s="11">
+        <f t="shared" si="7"/>
+        <v>152</v>
+      </c>
+      <c r="J21" s="41" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A22" s="3">
+        <f t="shared" si="5"/>
+        <v>20</v>
+      </c>
+      <c r="B22" s="11">
+        <f t="shared" si="7"/>
+        <v>167</v>
+      </c>
+      <c r="C22" s="11">
+        <f t="shared" si="7"/>
+        <v>166</v>
+      </c>
+      <c r="D22" s="11">
+        <f t="shared" si="7"/>
+        <v>165</v>
+      </c>
+      <c r="E22" s="11">
+        <f t="shared" si="7"/>
+        <v>164</v>
+      </c>
+      <c r="F22" s="11">
+        <f t="shared" si="7"/>
+        <v>163</v>
+      </c>
+      <c r="G22" s="11">
+        <f t="shared" si="7"/>
+        <v>162</v>
+      </c>
+      <c r="H22" s="11">
+        <f t="shared" si="7"/>
+        <v>161</v>
+      </c>
+      <c r="I22" s="11">
+        <f t="shared" si="7"/>
+        <v>160</v>
+      </c>
+      <c r="J22" s="41" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A23" s="3">
+        <f t="shared" si="5"/>
+        <v>21</v>
+      </c>
+      <c r="B23" s="11">
+        <f t="shared" si="7"/>
+        <v>175</v>
+      </c>
+      <c r="C23" s="11">
+        <f t="shared" si="7"/>
+        <v>174</v>
+      </c>
+      <c r="D23" s="11">
+        <f t="shared" si="7"/>
+        <v>173</v>
+      </c>
+      <c r="E23" s="11">
+        <f t="shared" si="7"/>
+        <v>172</v>
+      </c>
+      <c r="F23" s="11">
+        <f t="shared" si="7"/>
+        <v>171</v>
+      </c>
+      <c r="G23" s="11">
+        <f t="shared" si="7"/>
+        <v>170</v>
+      </c>
+      <c r="H23" s="11">
+        <f t="shared" si="7"/>
+        <v>169</v>
+      </c>
+      <c r="I23" s="11">
+        <f t="shared" si="7"/>
+        <v>168</v>
+      </c>
+      <c r="J23" s="41" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A24" s="3">
+        <f t="shared" si="5"/>
+        <v>22</v>
+      </c>
+      <c r="B24" s="11">
+        <f t="shared" si="7"/>
+        <v>183</v>
+      </c>
+      <c r="C24" s="11">
+        <f t="shared" si="7"/>
+        <v>182</v>
+      </c>
+      <c r="D24" s="11">
+        <f t="shared" si="7"/>
+        <v>181</v>
+      </c>
+      <c r="E24" s="11">
+        <f t="shared" si="7"/>
+        <v>180</v>
+      </c>
+      <c r="F24" s="11">
+        <f t="shared" si="7"/>
+        <v>179</v>
+      </c>
+      <c r="G24" s="11">
+        <f t="shared" si="7"/>
+        <v>178</v>
+      </c>
+      <c r="H24" s="11">
+        <f t="shared" si="7"/>
+        <v>177</v>
+      </c>
+      <c r="I24" s="11">
+        <f t="shared" si="7"/>
+        <v>176</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A25" s="3">
+        <f t="shared" si="5"/>
+        <v>23</v>
+      </c>
+      <c r="B25" s="11">
+        <f t="shared" si="7"/>
+        <v>191</v>
+      </c>
+      <c r="C25" s="11">
+        <f t="shared" si="7"/>
+        <v>190</v>
+      </c>
+      <c r="D25" s="11">
+        <f t="shared" si="7"/>
+        <v>189</v>
+      </c>
+      <c r="E25" s="11">
+        <f t="shared" si="7"/>
+        <v>188</v>
+      </c>
+      <c r="F25" s="11">
+        <f t="shared" si="7"/>
+        <v>187</v>
+      </c>
+      <c r="G25" s="11">
+        <f t="shared" si="7"/>
+        <v>186</v>
+      </c>
+      <c r="H25" s="11">
+        <f t="shared" si="7"/>
+        <v>185</v>
+      </c>
+      <c r="I25" s="11">
+        <f t="shared" si="7"/>
+        <v>184</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A26" s="3">
+        <f>A25+1</f>
+        <v>24</v>
+      </c>
+      <c r="B26" s="11">
+        <f t="shared" si="7"/>
+        <v>199</v>
+      </c>
+      <c r="C26" s="11">
+        <f t="shared" si="7"/>
+        <v>198</v>
+      </c>
+      <c r="D26" s="11">
+        <f t="shared" si="7"/>
+        <v>197</v>
+      </c>
+      <c r="E26" s="11">
+        <f t="shared" si="7"/>
+        <v>196</v>
+      </c>
+      <c r="F26" s="11">
+        <f t="shared" si="7"/>
+        <v>195</v>
+      </c>
+      <c r="G26" s="11">
+        <f t="shared" si="7"/>
+        <v>194</v>
+      </c>
+      <c r="H26" s="11">
+        <f t="shared" si="7"/>
+        <v>193</v>
+      </c>
+      <c r="I26" s="11">
+        <f t="shared" si="7"/>
+        <v>192</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A27" s="3">
+        <f t="shared" si="5"/>
+        <v>25</v>
+      </c>
+      <c r="B27" s="11">
+        <f t="shared" si="7"/>
+        <v>207</v>
+      </c>
+      <c r="C27" s="11">
+        <f t="shared" si="7"/>
+        <v>206</v>
+      </c>
+      <c r="D27" s="11">
+        <f t="shared" si="7"/>
+        <v>205</v>
+      </c>
+      <c r="E27" s="11">
+        <f t="shared" si="7"/>
+        <v>204</v>
+      </c>
+      <c r="F27" s="11">
+        <f t="shared" si="7"/>
+        <v>203</v>
+      </c>
+      <c r="G27" s="11">
+        <f t="shared" si="7"/>
+        <v>202</v>
+      </c>
+      <c r="H27" s="11">
+        <f t="shared" si="7"/>
+        <v>201</v>
+      </c>
+      <c r="I27" s="11">
+        <f t="shared" si="7"/>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A28" s="3">
+        <f t="shared" si="5"/>
+        <v>26</v>
+      </c>
+      <c r="B28" s="11">
+        <f t="shared" si="7"/>
+        <v>215</v>
+      </c>
+      <c r="C28" s="11">
+        <f t="shared" si="7"/>
+        <v>214</v>
+      </c>
+      <c r="D28" s="11">
+        <f t="shared" si="7"/>
+        <v>213</v>
+      </c>
+      <c r="E28" s="11">
+        <f t="shared" si="7"/>
+        <v>212</v>
+      </c>
+      <c r="F28" s="11">
+        <f t="shared" si="7"/>
+        <v>211</v>
+      </c>
+      <c r="G28" s="11">
+        <f t="shared" si="7"/>
+        <v>210</v>
+      </c>
+      <c r="H28" s="11">
+        <f t="shared" si="7"/>
+        <v>209</v>
+      </c>
+      <c r="I28" s="11">
+        <f t="shared" si="7"/>
+        <v>208</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A29" s="3">
+        <f t="shared" si="5"/>
+        <v>27</v>
+      </c>
+      <c r="B29" s="11">
+        <f t="shared" si="7"/>
+        <v>223</v>
+      </c>
+      <c r="C29" s="11">
+        <f t="shared" si="7"/>
+        <v>222</v>
+      </c>
+      <c r="D29" s="11">
+        <f t="shared" si="7"/>
+        <v>221</v>
+      </c>
+      <c r="E29" s="11">
+        <f t="shared" si="7"/>
+        <v>220</v>
+      </c>
+      <c r="F29" s="11">
+        <f t="shared" si="7"/>
+        <v>219</v>
+      </c>
+      <c r="G29" s="11">
+        <f t="shared" si="7"/>
+        <v>218</v>
+      </c>
+      <c r="H29" s="11">
+        <f t="shared" si="7"/>
+        <v>217</v>
+      </c>
+      <c r="I29" s="11">
+        <f t="shared" si="7"/>
+        <v>216</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A30" s="3">
+        <f t="shared" si="5"/>
+        <v>28</v>
+      </c>
+      <c r="B30" s="11">
+        <f t="shared" si="7"/>
+        <v>231</v>
+      </c>
+      <c r="C30" s="11">
+        <f t="shared" si="7"/>
+        <v>230</v>
+      </c>
+      <c r="D30" s="11">
+        <f t="shared" si="7"/>
+        <v>229</v>
+      </c>
+      <c r="E30" s="11">
+        <f t="shared" si="7"/>
+        <v>228</v>
+      </c>
+      <c r="F30" s="11">
+        <f t="shared" si="7"/>
+        <v>227</v>
+      </c>
+      <c r="G30" s="11">
+        <f t="shared" si="7"/>
+        <v>226</v>
+      </c>
+      <c r="H30" s="11">
+        <f t="shared" si="7"/>
+        <v>225</v>
+      </c>
+      <c r="I30" s="11">
+        <f t="shared" si="7"/>
+        <v>224</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A31" s="3">
+        <f t="shared" si="5"/>
+        <v>29</v>
+      </c>
+      <c r="B31" s="11">
+        <f t="shared" si="7"/>
+        <v>239</v>
+      </c>
+      <c r="C31" s="11">
+        <f t="shared" si="7"/>
+        <v>238</v>
+      </c>
+      <c r="D31" s="11">
+        <f t="shared" si="7"/>
+        <v>237</v>
+      </c>
+      <c r="E31" s="11">
+        <f t="shared" si="7"/>
+        <v>236</v>
+      </c>
+      <c r="F31" s="11">
+        <f t="shared" si="7"/>
+        <v>235</v>
+      </c>
+      <c r="G31" s="11">
+        <f t="shared" si="7"/>
+        <v>234</v>
+      </c>
+      <c r="H31" s="11">
+        <f t="shared" si="7"/>
+        <v>233</v>
+      </c>
+      <c r="I31" s="11">
+        <f t="shared" si="7"/>
+        <v>232</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A32" s="3">
+        <f>A31+1</f>
+        <v>30</v>
+      </c>
+      <c r="B32" s="11">
+        <f t="shared" si="7"/>
+        <v>247</v>
+      </c>
+      <c r="C32" s="11">
+        <f t="shared" si="7"/>
+        <v>246</v>
+      </c>
+      <c r="D32" s="11">
+        <f t="shared" si="7"/>
+        <v>245</v>
+      </c>
+      <c r="E32" s="11">
+        <f t="shared" si="7"/>
+        <v>244</v>
+      </c>
+      <c r="F32" s="11">
+        <f t="shared" si="7"/>
+        <v>243</v>
+      </c>
+      <c r="G32" s="11">
+        <f t="shared" si="7"/>
+        <v>242</v>
+      </c>
+      <c r="H32" s="11">
+        <f t="shared" si="7"/>
+        <v>241</v>
+      </c>
+      <c r="I32" s="11">
+        <f t="shared" si="7"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="3">
+        <f t="shared" si="5"/>
+        <v>31</v>
+      </c>
+      <c r="B33" s="11">
+        <f t="shared" si="7"/>
+        <v>255</v>
+      </c>
+      <c r="C33" s="11">
+        <f t="shared" si="7"/>
+        <v>254</v>
+      </c>
+      <c r="D33" s="11">
+        <f t="shared" si="7"/>
+        <v>253</v>
+      </c>
+      <c r="E33" s="11">
+        <f t="shared" si="7"/>
+        <v>252</v>
+      </c>
+      <c r="F33" s="11">
+        <f t="shared" si="7"/>
+        <v>251</v>
+      </c>
+      <c r="G33" s="11">
+        <f t="shared" si="7"/>
+        <v>250</v>
+      </c>
+      <c r="H33" s="11">
+        <f t="shared" si="7"/>
+        <v>249</v>
+      </c>
+      <c r="I33" s="11">
+        <f t="shared" si="7"/>
+        <v>248</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="16">
+    <mergeCell ref="J14:Q14"/>
+    <mergeCell ref="J15:Q15"/>
+    <mergeCell ref="J16:Q16"/>
+    <mergeCell ref="J17:Q17"/>
+    <mergeCell ref="J8:Q8"/>
+    <mergeCell ref="J9:Q9"/>
+    <mergeCell ref="J10:Q10"/>
+    <mergeCell ref="J11:Q11"/>
+    <mergeCell ref="J12:Q12"/>
+    <mergeCell ref="J13:Q13"/>
+    <mergeCell ref="J2:Q2"/>
+    <mergeCell ref="J3:Q3"/>
+    <mergeCell ref="J4:Q4"/>
+    <mergeCell ref="J5:Q5"/>
+    <mergeCell ref="J6:Q6"/>
+    <mergeCell ref="J7:Q7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B0846F3-C267-499B-9941-B9FBFB633FBE}">
   <dimension ref="A1:D25"/>
   <sheetViews>
@@ -1059,11 +3094,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52ED2EEC-F36A-4A8D-A22A-BD01CD04C3CE}">
   <dimension ref="A1:K65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A18" sqref="A18:XFD18"/>
     </sheetView>
@@ -3448,7 +5483,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{804CB660-8CFB-4F70-B751-D2BBCE3FAF4B}">
   <dimension ref="A1:C7"/>
   <sheetViews>

</xml_diff>

<commit_message>
Added double height, blast through and flash.
</commit_message>
<xml_diff>
--- a/docs/control codes.xlsx
+++ b/docs/control codes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robin\Documents\Visual Studio 2015\Projects\NexTel\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C888221-73A8-423D-8251-4913A6BE69BB}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{179CD669-A1C3-4BAD-9F5A-AF33AD546EA9}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16695" windowHeight="5955" xr2:uid="{1D35677F-1048-41AB-9A0D-5C34EC10B2B0}"/>
   </bookViews>
@@ -327,10 +327,10 @@
     <t>Palette indices 136..255 are not used, except $E3 which is transparent (for box mode support)</t>
   </si>
   <si>
-    <t>Conceal/Reveal is implemented by substituting Conceal $98 for Escape $9B (or vice-versa) in the buffer, then re-rendering</t>
-  </si>
-  <si>
-    <t>Box mode is implemented by rendering with a branch to draw transparent FG and BG when outside box</t>
+    <t>Box mode is implemented by (re)rendering with a branch to draw transparent FG and BG when outside box</t>
+  </si>
+  <si>
+    <t>Conceal/Reveal is implemented by substituting Conceal $98 for Escape $9B (or vice-versa) in the buffer, then (re)rendering</t>
   </si>
 </sst>
 </file>
@@ -601,30 +601,6 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -660,6 +636,30 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -988,14 +988,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E06C7C1-2502-41BC-8AA4-E8D6C1F363EE}">
   <dimension ref="A1:W33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="J23" sqref="J23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="9" width="4" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="17" width="11.85546875" style="1" customWidth="1"/>
-    <col min="18" max="19" width="9" style="39" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="9" style="31" bestFit="1" customWidth="1"/>
     <col min="20" max="23" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -1056,10 +1058,10 @@
       <c r="Q1" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="R1" s="30" t="s">
+      <c r="R1" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="S1" s="30" t="s">
+      <c r="S1" s="22" t="s">
         <v>85</v>
       </c>
       <c r="T1" s="10" t="s">
@@ -1111,21 +1113,21 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J2" s="22" t="s">
+      <c r="J2" s="38" t="s">
         <v>68</v>
       </c>
-      <c r="K2" s="22"/>
-      <c r="L2" s="22"/>
-      <c r="M2" s="22"/>
-      <c r="N2" s="22"/>
-      <c r="O2" s="22"/>
-      <c r="P2" s="22"/>
-      <c r="Q2" s="22"/>
-      <c r="R2" s="39" t="str">
+      <c r="K2" s="38"/>
+      <c r="L2" s="38"/>
+      <c r="M2" s="38"/>
+      <c r="N2" s="38"/>
+      <c r="O2" s="38"/>
+      <c r="P2" s="38"/>
+      <c r="Q2" s="38"/>
+      <c r="R2" s="31" t="str">
         <f>DEC2BIN(B2, 8)</f>
         <v>00000111</v>
       </c>
-      <c r="S2" s="39" t="str">
+      <c r="S2" s="31" t="str">
         <f>DEC2BIN(I2, 8)</f>
         <v>00000000</v>
       </c>
@@ -1179,21 +1181,21 @@
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="J3" s="23" t="s">
+      <c r="J3" s="39" t="s">
         <v>69</v>
       </c>
-      <c r="K3" s="23"/>
-      <c r="L3" s="23"/>
-      <c r="M3" s="23"/>
-      <c r="N3" s="23"/>
-      <c r="O3" s="23"/>
-      <c r="P3" s="23"/>
-      <c r="Q3" s="23"/>
-      <c r="R3" s="39" t="str">
+      <c r="K3" s="39"/>
+      <c r="L3" s="39"/>
+      <c r="M3" s="39"/>
+      <c r="N3" s="39"/>
+      <c r="O3" s="39"/>
+      <c r="P3" s="39"/>
+      <c r="Q3" s="39"/>
+      <c r="R3" s="31" t="str">
         <f t="shared" ref="R3:R18" si="3">DEC2BIN(B3, 8)</f>
         <v>00001111</v>
       </c>
-      <c r="S3" s="39" t="str">
+      <c r="S3" s="31" t="str">
         <f t="shared" ref="S3:S18" si="4">DEC2BIN(I3, 8)</f>
         <v>00001000</v>
       </c>
@@ -1235,21 +1237,21 @@
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="J4" s="24" t="s">
+      <c r="J4" s="40" t="s">
         <v>70</v>
       </c>
-      <c r="K4" s="24"/>
-      <c r="L4" s="24"/>
-      <c r="M4" s="24"/>
-      <c r="N4" s="24"/>
-      <c r="O4" s="24"/>
-      <c r="P4" s="24"/>
-      <c r="Q4" s="24"/>
-      <c r="R4" s="39" t="str">
+      <c r="K4" s="40"/>
+      <c r="L4" s="40"/>
+      <c r="M4" s="40"/>
+      <c r="N4" s="40"/>
+      <c r="O4" s="40"/>
+      <c r="P4" s="40"/>
+      <c r="Q4" s="40"/>
+      <c r="R4" s="31" t="str">
         <f t="shared" si="3"/>
         <v>00010111</v>
       </c>
-      <c r="S4" s="39" t="str">
+      <c r="S4" s="31" t="str">
         <f t="shared" si="4"/>
         <v>00010000</v>
       </c>
@@ -1291,21 +1293,21 @@
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="J5" s="25" t="s">
+      <c r="J5" s="41" t="s">
         <v>71</v>
       </c>
-      <c r="K5" s="25"/>
-      <c r="L5" s="25"/>
-      <c r="M5" s="25"/>
-      <c r="N5" s="25"/>
-      <c r="O5" s="25"/>
-      <c r="P5" s="25"/>
-      <c r="Q5" s="25"/>
-      <c r="R5" s="39" t="str">
+      <c r="K5" s="41"/>
+      <c r="L5" s="41"/>
+      <c r="M5" s="41"/>
+      <c r="N5" s="41"/>
+      <c r="O5" s="41"/>
+      <c r="P5" s="41"/>
+      <c r="Q5" s="41"/>
+      <c r="R5" s="31" t="str">
         <f t="shared" si="3"/>
         <v>00011111</v>
       </c>
-      <c r="S5" s="39" t="str">
+      <c r="S5" s="31" t="str">
         <f t="shared" si="4"/>
         <v>00011000</v>
       </c>
@@ -1347,21 +1349,21 @@
         <f t="shared" si="1"/>
         <v>32</v>
       </c>
-      <c r="J6" s="26" t="s">
+      <c r="J6" s="34" t="s">
         <v>72</v>
       </c>
-      <c r="K6" s="26"/>
-      <c r="L6" s="26"/>
-      <c r="M6" s="26"/>
-      <c r="N6" s="26"/>
-      <c r="O6" s="26"/>
-      <c r="P6" s="26"/>
-      <c r="Q6" s="26"/>
-      <c r="R6" s="39" t="str">
+      <c r="K6" s="34"/>
+      <c r="L6" s="34"/>
+      <c r="M6" s="34"/>
+      <c r="N6" s="34"/>
+      <c r="O6" s="34"/>
+      <c r="P6" s="34"/>
+      <c r="Q6" s="34"/>
+      <c r="R6" s="31" t="str">
         <f t="shared" si="3"/>
         <v>00100111</v>
       </c>
-      <c r="S6" s="39" t="str">
+      <c r="S6" s="31" t="str">
         <f t="shared" si="4"/>
         <v>00100000</v>
       </c>
@@ -1403,21 +1405,21 @@
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
-      <c r="J7" s="27" t="s">
+      <c r="J7" s="35" t="s">
         <v>73</v>
       </c>
-      <c r="K7" s="27"/>
-      <c r="L7" s="27"/>
-      <c r="M7" s="27"/>
-      <c r="N7" s="27"/>
-      <c r="O7" s="27"/>
-      <c r="P7" s="27"/>
-      <c r="Q7" s="27"/>
-      <c r="R7" s="39" t="str">
+      <c r="K7" s="35"/>
+      <c r="L7" s="35"/>
+      <c r="M7" s="35"/>
+      <c r="N7" s="35"/>
+      <c r="O7" s="35"/>
+      <c r="P7" s="35"/>
+      <c r="Q7" s="35"/>
+      <c r="R7" s="31" t="str">
         <f t="shared" si="3"/>
         <v>00101111</v>
       </c>
-      <c r="S7" s="39" t="str">
+      <c r="S7" s="31" t="str">
         <f t="shared" si="4"/>
         <v>00101000</v>
       </c>
@@ -1459,21 +1461,21 @@
         <f t="shared" si="1"/>
         <v>48</v>
       </c>
-      <c r="J8" s="28" t="s">
+      <c r="J8" s="36" t="s">
         <v>74</v>
       </c>
-      <c r="K8" s="28"/>
-      <c r="L8" s="28"/>
-      <c r="M8" s="28"/>
-      <c r="N8" s="28"/>
-      <c r="O8" s="28"/>
-      <c r="P8" s="28"/>
-      <c r="Q8" s="28"/>
-      <c r="R8" s="39" t="str">
+      <c r="K8" s="36"/>
+      <c r="L8" s="36"/>
+      <c r="M8" s="36"/>
+      <c r="N8" s="36"/>
+      <c r="O8" s="36"/>
+      <c r="P8" s="36"/>
+      <c r="Q8" s="36"/>
+      <c r="R8" s="31" t="str">
         <f t="shared" si="3"/>
         <v>00110111</v>
       </c>
-      <c r="S8" s="39" t="str">
+      <c r="S8" s="31" t="str">
         <f t="shared" si="4"/>
         <v>00110000</v>
       </c>
@@ -1515,21 +1517,21 @@
         <f t="shared" si="1"/>
         <v>56</v>
       </c>
-      <c r="J9" s="29" t="s">
+      <c r="J9" s="37" t="s">
         <v>75</v>
       </c>
-      <c r="K9" s="29"/>
-      <c r="L9" s="29"/>
-      <c r="M9" s="29"/>
-      <c r="N9" s="29"/>
-      <c r="O9" s="29"/>
-      <c r="P9" s="29"/>
-      <c r="Q9" s="29"/>
-      <c r="R9" s="39" t="str">
+      <c r="K9" s="37"/>
+      <c r="L9" s="37"/>
+      <c r="M9" s="37"/>
+      <c r="N9" s="37"/>
+      <c r="O9" s="37"/>
+      <c r="P9" s="37"/>
+      <c r="Q9" s="37"/>
+      <c r="R9" s="31" t="str">
         <f t="shared" si="3"/>
         <v>00111111</v>
       </c>
-      <c r="S9" s="39" t="str">
+      <c r="S9" s="31" t="str">
         <f t="shared" si="4"/>
         <v>00111000</v>
       </c>
@@ -1571,21 +1573,21 @@
         <f t="shared" si="1"/>
         <v>64</v>
       </c>
-      <c r="J10" s="22" t="s">
+      <c r="J10" s="38" t="s">
         <v>76</v>
       </c>
-      <c r="K10" s="22"/>
-      <c r="L10" s="22"/>
-      <c r="M10" s="22"/>
-      <c r="N10" s="22"/>
-      <c r="O10" s="22"/>
-      <c r="P10" s="22"/>
-      <c r="Q10" s="22"/>
-      <c r="R10" s="39" t="str">
+      <c r="K10" s="38"/>
+      <c r="L10" s="38"/>
+      <c r="M10" s="38"/>
+      <c r="N10" s="38"/>
+      <c r="O10" s="38"/>
+      <c r="P10" s="38"/>
+      <c r="Q10" s="38"/>
+      <c r="R10" s="31" t="str">
         <f t="shared" si="3"/>
         <v>01000111</v>
       </c>
-      <c r="S10" s="39" t="str">
+      <c r="S10" s="31" t="str">
         <f t="shared" si="4"/>
         <v>01000000</v>
       </c>
@@ -1627,21 +1629,21 @@
         <f t="shared" si="1"/>
         <v>72</v>
       </c>
-      <c r="J11" s="23" t="s">
+      <c r="J11" s="39" t="s">
         <v>77</v>
       </c>
-      <c r="K11" s="23"/>
-      <c r="L11" s="23"/>
-      <c r="M11" s="23"/>
-      <c r="N11" s="23"/>
-      <c r="O11" s="23"/>
-      <c r="P11" s="23"/>
-      <c r="Q11" s="23"/>
-      <c r="R11" s="39" t="str">
+      <c r="K11" s="39"/>
+      <c r="L11" s="39"/>
+      <c r="M11" s="39"/>
+      <c r="N11" s="39"/>
+      <c r="O11" s="39"/>
+      <c r="P11" s="39"/>
+      <c r="Q11" s="39"/>
+      <c r="R11" s="31" t="str">
         <f t="shared" si="3"/>
         <v>01001111</v>
       </c>
-      <c r="S11" s="39" t="str">
+      <c r="S11" s="31" t="str">
         <f t="shared" si="4"/>
         <v>01001000</v>
       </c>
@@ -1683,21 +1685,21 @@
         <f t="shared" si="1"/>
         <v>80</v>
       </c>
-      <c r="J12" s="24" t="s">
+      <c r="J12" s="40" t="s">
         <v>78</v>
       </c>
-      <c r="K12" s="24"/>
-      <c r="L12" s="24"/>
-      <c r="M12" s="24"/>
-      <c r="N12" s="24"/>
-      <c r="O12" s="24"/>
-      <c r="P12" s="24"/>
-      <c r="Q12" s="24"/>
-      <c r="R12" s="39" t="str">
+      <c r="K12" s="40"/>
+      <c r="L12" s="40"/>
+      <c r="M12" s="40"/>
+      <c r="N12" s="40"/>
+      <c r="O12" s="40"/>
+      <c r="P12" s="40"/>
+      <c r="Q12" s="40"/>
+      <c r="R12" s="31" t="str">
         <f t="shared" si="3"/>
         <v>01010111</v>
       </c>
-      <c r="S12" s="39" t="str">
+      <c r="S12" s="31" t="str">
         <f t="shared" si="4"/>
         <v>01010000</v>
       </c>
@@ -1739,21 +1741,21 @@
         <f t="shared" si="1"/>
         <v>88</v>
       </c>
-      <c r="J13" s="25" t="s">
+      <c r="J13" s="41" t="s">
         <v>79</v>
       </c>
-      <c r="K13" s="25"/>
-      <c r="L13" s="25"/>
-      <c r="M13" s="25"/>
-      <c r="N13" s="25"/>
-      <c r="O13" s="25"/>
-      <c r="P13" s="25"/>
-      <c r="Q13" s="25"/>
-      <c r="R13" s="39" t="str">
+      <c r="K13" s="41"/>
+      <c r="L13" s="41"/>
+      <c r="M13" s="41"/>
+      <c r="N13" s="41"/>
+      <c r="O13" s="41"/>
+      <c r="P13" s="41"/>
+      <c r="Q13" s="41"/>
+      <c r="R13" s="31" t="str">
         <f t="shared" si="3"/>
         <v>01011111</v>
       </c>
-      <c r="S13" s="39" t="str">
+      <c r="S13" s="31" t="str">
         <f t="shared" si="4"/>
         <v>01011000</v>
       </c>
@@ -1795,21 +1797,21 @@
         <f t="shared" si="1"/>
         <v>96</v>
       </c>
-      <c r="J14" s="26" t="s">
+      <c r="J14" s="34" t="s">
         <v>80</v>
       </c>
-      <c r="K14" s="26"/>
-      <c r="L14" s="26"/>
-      <c r="M14" s="26"/>
-      <c r="N14" s="26"/>
-      <c r="O14" s="26"/>
-      <c r="P14" s="26"/>
-      <c r="Q14" s="26"/>
-      <c r="R14" s="39" t="str">
+      <c r="K14" s="34"/>
+      <c r="L14" s="34"/>
+      <c r="M14" s="34"/>
+      <c r="N14" s="34"/>
+      <c r="O14" s="34"/>
+      <c r="P14" s="34"/>
+      <c r="Q14" s="34"/>
+      <c r="R14" s="31" t="str">
         <f t="shared" si="3"/>
         <v>01100111</v>
       </c>
-      <c r="S14" s="39" t="str">
+      <c r="S14" s="31" t="str">
         <f t="shared" si="4"/>
         <v>01100000</v>
       </c>
@@ -1851,21 +1853,21 @@
         <f t="shared" si="1"/>
         <v>104</v>
       </c>
-      <c r="J15" s="27" t="s">
+      <c r="J15" s="35" t="s">
         <v>81</v>
       </c>
-      <c r="K15" s="27"/>
-      <c r="L15" s="27"/>
-      <c r="M15" s="27"/>
-      <c r="N15" s="27"/>
-      <c r="O15" s="27"/>
-      <c r="P15" s="27"/>
-      <c r="Q15" s="27"/>
-      <c r="R15" s="39" t="str">
+      <c r="K15" s="35"/>
+      <c r="L15" s="35"/>
+      <c r="M15" s="35"/>
+      <c r="N15" s="35"/>
+      <c r="O15" s="35"/>
+      <c r="P15" s="35"/>
+      <c r="Q15" s="35"/>
+      <c r="R15" s="31" t="str">
         <f t="shared" si="3"/>
         <v>01101111</v>
       </c>
-      <c r="S15" s="39" t="str">
+      <c r="S15" s="31" t="str">
         <f t="shared" si="4"/>
         <v>01101000</v>
       </c>
@@ -1907,21 +1909,21 @@
         <f t="shared" si="1"/>
         <v>112</v>
       </c>
-      <c r="J16" s="28" t="s">
+      <c r="J16" s="36" t="s">
         <v>82</v>
       </c>
-      <c r="K16" s="28"/>
-      <c r="L16" s="28"/>
-      <c r="M16" s="28"/>
-      <c r="N16" s="28"/>
-      <c r="O16" s="28"/>
-      <c r="P16" s="28"/>
-      <c r="Q16" s="28"/>
-      <c r="R16" s="39" t="str">
+      <c r="K16" s="36"/>
+      <c r="L16" s="36"/>
+      <c r="M16" s="36"/>
+      <c r="N16" s="36"/>
+      <c r="O16" s="36"/>
+      <c r="P16" s="36"/>
+      <c r="Q16" s="36"/>
+      <c r="R16" s="31" t="str">
         <f t="shared" si="3"/>
         <v>01110111</v>
       </c>
-      <c r="S16" s="39" t="str">
+      <c r="S16" s="31" t="str">
         <f t="shared" si="4"/>
         <v>01110000</v>
       </c>
@@ -1963,21 +1965,21 @@
         <f t="shared" si="1"/>
         <v>120</v>
       </c>
-      <c r="J17" s="29" t="s">
+      <c r="J17" s="37" t="s">
         <v>83</v>
       </c>
-      <c r="K17" s="29"/>
-      <c r="L17" s="29"/>
-      <c r="M17" s="29"/>
-      <c r="N17" s="29"/>
-      <c r="O17" s="29"/>
-      <c r="P17" s="29"/>
-      <c r="Q17" s="29"/>
-      <c r="R17" s="39" t="str">
+      <c r="K17" s="37"/>
+      <c r="L17" s="37"/>
+      <c r="M17" s="37"/>
+      <c r="N17" s="37"/>
+      <c r="O17" s="37"/>
+      <c r="P17" s="37"/>
+      <c r="Q17" s="37"/>
+      <c r="R17" s="31" t="str">
         <f t="shared" si="3"/>
         <v>01111111</v>
       </c>
-      <c r="S17" s="39" t="str">
+      <c r="S17" s="31" t="str">
         <f t="shared" si="4"/>
         <v>01111000</v>
       </c>
@@ -2019,43 +2021,43 @@
         <f t="shared" si="2"/>
         <v>128</v>
       </c>
-      <c r="J18" s="31" t="str">
+      <c r="J18" s="23" t="str">
         <f>J$1 &amp; " BG"</f>
         <v>White BG</v>
       </c>
-      <c r="K18" s="32" t="str">
+      <c r="K18" s="24" t="str">
         <f t="shared" ref="K18:Q18" si="6">K$1 &amp; " BG"</f>
         <v>Cyan BG</v>
       </c>
-      <c r="L18" s="33" t="str">
+      <c r="L18" s="25" t="str">
         <f t="shared" si="6"/>
         <v>Magenta BG</v>
       </c>
-      <c r="M18" s="34" t="str">
+      <c r="M18" s="26" t="str">
         <f t="shared" si="6"/>
         <v>Blue BG</v>
       </c>
-      <c r="N18" s="35" t="str">
+      <c r="N18" s="27" t="str">
         <f t="shared" si="6"/>
         <v>Yellow BG</v>
       </c>
-      <c r="O18" s="36" t="str">
+      <c r="O18" s="28" t="str">
         <f t="shared" si="6"/>
         <v>Green BG</v>
       </c>
-      <c r="P18" s="37" t="str">
+      <c r="P18" s="29" t="str">
         <f t="shared" si="6"/>
         <v>Red BG</v>
       </c>
-      <c r="Q18" s="38" t="str">
+      <c r="Q18" s="30" t="str">
         <f t="shared" si="6"/>
         <v>Black BG</v>
       </c>
-      <c r="R18" s="39" t="str">
+      <c r="R18" s="31" t="str">
         <f t="shared" si="3"/>
         <v>10000111</v>
       </c>
-      <c r="S18" s="39" t="str">
+      <c r="S18" s="31" t="str">
         <f t="shared" si="4"/>
         <v>10000000</v>
       </c>
@@ -2097,10 +2099,10 @@
         <f t="shared" si="7"/>
         <v>136</v>
       </c>
-      <c r="J19" s="40" t="s">
+      <c r="J19" s="32" t="s">
         <v>94</v>
       </c>
-      <c r="K19" s="41" t="s">
+      <c r="K19" s="33" t="s">
         <v>96</v>
       </c>
     </row>
@@ -2141,10 +2143,10 @@
         <f t="shared" si="7"/>
         <v>144</v>
       </c>
-      <c r="J20" s="40" t="s">
+      <c r="J20" s="32" t="s">
         <v>95</v>
       </c>
-      <c r="K20" s="41" t="s">
+      <c r="K20" s="33" t="s">
         <v>97</v>
       </c>
     </row>
@@ -2185,7 +2187,7 @@
         <f t="shared" si="7"/>
         <v>152</v>
       </c>
-      <c r="J21" s="41" t="s">
+      <c r="J21" s="33" t="s">
         <v>98</v>
       </c>
     </row>
@@ -2226,8 +2228,8 @@
         <f t="shared" si="7"/>
         <v>160</v>
       </c>
-      <c r="J22" s="41" t="s">
-        <v>99</v>
+      <c r="J22" s="33" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
@@ -2267,8 +2269,8 @@
         <f t="shared" si="7"/>
         <v>168</v>
       </c>
-      <c r="J23" s="41" t="s">
-        <v>100</v>
+      <c r="J23" s="33" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
@@ -2653,6 +2655,12 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="J7:Q7"/>
+    <mergeCell ref="J2:Q2"/>
+    <mergeCell ref="J3:Q3"/>
+    <mergeCell ref="J4:Q4"/>
+    <mergeCell ref="J5:Q5"/>
+    <mergeCell ref="J6:Q6"/>
     <mergeCell ref="J14:Q14"/>
     <mergeCell ref="J15:Q15"/>
     <mergeCell ref="J16:Q16"/>
@@ -2663,12 +2671,6 @@
     <mergeCell ref="J11:Q11"/>
     <mergeCell ref="J12:Q12"/>
     <mergeCell ref="J13:Q13"/>
-    <mergeCell ref="J2:Q2"/>
-    <mergeCell ref="J3:Q3"/>
-    <mergeCell ref="J4:Q4"/>
-    <mergeCell ref="J5:Q5"/>
-    <mergeCell ref="J6:Q6"/>
-    <mergeCell ref="J7:Q7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>